<commit_message>
Change of write_to_excel for output cost combination
</commit_message>
<xml_diff>
--- a/data/input/tree/meaningfulness/ecology/ecosystems.xlsx
+++ b/data/input/tree/meaningfulness/ecology/ecosystems.xlsx
@@ -447,7 +447,7 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>1</v>
+        <v>0.7615595611285266</v>
       </c>
     </row>
     <row r="3">
@@ -457,7 +457,7 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>0.7607913669064748</v>
+        <v>0.6871081504702194</v>
       </c>
     </row>
     <row r="4">
@@ -467,7 +467,7 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>0.9694244604316546</v>
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>